<commit_message>
update test cases _STA
</commit_message>
<xml_diff>
--- a/Test Documentation/Test Cases/Web_app/TestCases for learn.epam.com _STA course.xlsx
+++ b/Test Documentation/Test Cases/Web_app/TestCases for learn.epam.com _STA course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\Portfolio_Tester\Test Documentation\Test Cases\Web_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E3E17FC-A098-4187-B4FA-C6BA7B819BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225B760A-AD32-4ABA-9806-B5DC8FEAC9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-4430" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35940" yWindow="-4320" windowWidth="15870" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_cases_Smoke_learn.epam.com" sheetId="2" r:id="rId1"/>
@@ -93,13 +93,6 @@
 5. Click on the "Log in to get full experience" button.</t>
   </si>
   <si>
-    <t>1.  The "Log in" button is presented in the right corner of the Main Menu before the "Public App" widget.
-2.  The "Log in" button is presented in the on the Start page header on the right.
-3. The user is redirected to the EPAM Digital Platform (https://access.epam.com/auth/....) for further login.
-4. The user is on the Start page again.
-5. The user is redirected to the EPAM Digital Platform (https://access.epam.com/auth/....) for further login.</t>
-  </si>
-  <si>
     <t>1. The user hasn't logged in to the application yet.
 2. The user is in on the Base Details Page of any course except those courses that does not require registration.</t>
   </si>
@@ -132,14 +125,7 @@
 4. The user is redirected to the EPAM Digital Platform (https://access.epam.com/auth/....) for further login.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sign out </t>
-  </si>
-  <si>
     <t>1. The user is logged in to the application.</t>
-  </si>
-  <si>
-    <t>1. Click on the Avatar (Profile icon) located in the Main Menu.
-2. Click on the "Sign out" button at the end of  Dropdown menu.</t>
   </si>
   <si>
     <t>Content</t>
@@ -171,12 +157,6 @@
 2. The user is on Base Details Page of any course, that not requires registration of participants.</t>
   </si>
   <si>
-    <t>1. Check the presence of two  "Study" buttons on the Base Details Page of course.
-2. Click on the "Study" button on the header of this page.
-3. Return on the Base Details Page of course.
-4. Click on the "Study" button in the "Summary" widget on this page.</t>
-  </si>
-  <si>
     <t>1. There are two "Study" buttons on the Base Details Page.
 2. The user is redirected to the eLearn.EPAM.com platform with this course.
 3. The user is on the Base Details Page of this course again.
@@ -209,6 +189,26 @@
   <si>
     <t>1. The dropdown menu of the Avatar opened.
 2. The user has signed out.</t>
+  </si>
+  <si>
+    <t>Sign out</t>
+  </si>
+  <si>
+    <t>1. The "Log in" button is presented in the right corner of the Main Menu before the "Public App" widget.
+2. The "Log in" button is presented in the on the Start page header on the right.
+3. The user is redirected to the EPAM Digital Platform (https://access.epam.com/auth/....) for further login.
+4. The user is on the Start page again.
+5. The user is redirected to the EPAM Digital Platform (https://access.epam.com/auth/....) for further login.</t>
+  </si>
+  <si>
+    <t>1. Click on the Avatar (Profile icon) located in the Main Menu.
+2. Click on the "Sign out" button at the end of Dropdown menu.</t>
+  </si>
+  <si>
+    <t>1. Check the presence of two "Study" buttons on the Base Details Page of course.
+2. Click on the "Study" button on the header of this page.
+3. Return on the Base Details Page of course.
+4. Click on the "Study" button in the "Summary" widget on this page.</t>
   </si>
 </sst>
 </file>
@@ -394,6 +394,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -408,12 +414,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -754,34 +754,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="A1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="A2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
@@ -819,7 +819,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="140.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
+      <c r="A4" s="13">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -835,7 +835,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>15</v>
@@ -844,13 +844,13 @@
         <v>16</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+      <c r="A5" s="14">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -866,22 +866,22 @@
         <v>14</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
+      <c r="A6" s="13">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -897,22 +897,22 @@
         <v>14</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
+      <c r="A7" s="14">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -925,25 +925,25 @@
         <v>13</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="A8" s="13">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -953,28 +953,28 @@
         <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+      <c r="A9" s="14">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -984,38 +984,38 @@
         <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1025,7 +1025,6 @@
     <mergeCell ref="A2:K2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F4" location="'1-2q_Checklist'!F9" display="presence and work of &quot;Log in&quot; buttons on Start page " xr:uid="{06C43D49-FF47-4AEB-8AB2-0AA98ED37DEF}"/>
     <hyperlink ref="A2:K2" r:id="rId1" display="Back on main page" xr:uid="{A1B9ED90-C95D-40DC-932C-F02DF8C1CC04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>